<commit_message>
Data, scripts, and packages for managing gas data and calculating k600.
</commit_message>
<xml_diff>
--- a/SuRGE_Sharepoint/data/CIN/CH4_207_old mans lake/dataSheets/surgeData207.xlsx
+++ b/SuRGE_Sharepoint/data/CIN/CH4_207_old mans lake/dataSheets/surgeData207.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/beaulieu_jake_epa_gov/Documents/gitRepository/SuRGE/SuRGE_Sharepoint/data/CIN/CH4_207_old mans lake/dataSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="807" documentId="8_{574317AD-36CA-42B2-83FE-C04BF0299D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6811ADCD-12F8-4CDB-9352-999A5AC858A4}"/>
+  <xr:revisionPtr revIDLastSave="808" documentId="8_{574317AD-36CA-42B2-83FE-C04BF0299D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55AA5A50-8234-4D4B-BBCA-26315F0DA671}"/>
   <bookViews>
-    <workbookView xWindow="22944" yWindow="0" windowWidth="23232" windowHeight="18576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1610,7 +1610,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="AK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BA17" sqref="BA17"/>
+      <selection pane="topRight" activeCell="AQ17" sqref="AQ17:AT17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2983,15 +2983,6 @@
       <c r="AN17" t="s">
         <v>175</v>
       </c>
-      <c r="AQ17">
-        <v>13.4</v>
-      </c>
-      <c r="AR17">
-        <v>9.4</v>
-      </c>
-      <c r="AS17">
-        <v>0</v>
-      </c>
       <c r="BJ17" t="s">
         <v>176</v>
       </c>
@@ -4084,57 +4075,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
-    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
-    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-10-21T13:32:44+00:00</Document_x0020_Creation_x0020_Date>
-    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j747ac98061d40f0aa7bd47e1db5675d>
-    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Creator>
-    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </EPA_x0020_Contributor>
-    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed970698-2d60-4bab-a048-d9be527522d9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001AF5FC5DD832BE4DBA6B24560DD3ADC0" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d9110ddba8137efcfc9b628571238300">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="8b03727f-4454-4722-b3e6-018d8dcaf2fd" xmlns:ns6="ed970698-2d60-4bab-a048-d9be527522d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bebf8e6f5f0ff6ff908ec6e1ee4006f7" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4599,34 +4539,63 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-10-21T13:32:44+00:00</Document_x0020_Creation_x0020_Date>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j747ac98061d40f0aa7bd47e1db5675d>
+    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Creator>
+    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </EPA_x0020_Contributor>
+    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed970698-2d60-4bab-a048-d9be527522d9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F4A5FCF-4499-487A-89B0-E215184C11DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D26D44A-9508-4707-B138-18882E5BA6FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="ed970698-2d60-4bab-a048-d9be527522d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FA34717-D6CC-4CD4-B8FC-9B0228131B2D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4649,6 +4618,28 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D26D44A-9508-4707-B138-18882E5BA6FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="ed970698-2d60-4bab-a048-d9be527522d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F4A5FCF-4499-487A-89B0-E215184C11DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845EA28A-135D-4CD8-9991-40FEAFECD172}">
   <ds:schemaRefs>

</xml_diff>